<commit_message>
Missing summary total qty in report_stock_summary
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/stock_summary.xlsx
+++ b/netforce_stock/netforce_stock/reports/stock_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,16 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Stock Summary</t>
   </si>
@@ -106,13 +111,25 @@
     <t>{{/each}}</t>
   </si>
   <si>
+    <t>{{currency total_open_qty}}</t>
+  </si>
+  <si>
     <t>{{currency total_open_amt}}</t>
   </si>
   <si>
+    <t>{{currency total_period_in_qty}}</t>
+  </si>
+  <si>
     <t>{{currency total_period_in_amt}}</t>
   </si>
   <si>
+    <t>{{currency total_period_out_qty}}</t>
+  </si>
+  <si>
     <t>{{currency total_period_out_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency total_close_qty}}</t>
   </si>
   <si>
     <t>{{currency total_close_amt}}</t>
@@ -197,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +229,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -229,27 +254,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="19.9234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.9081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.9081632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -388,17 +413,29 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="G11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="H11" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -426,7 +463,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -437,7 +474,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -453,7 +490,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -464,7 +501,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add brand in report stock summary
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/stock_summary.xlsx
+++ b/netforce_stock/netforce_stock/reports/stock_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,165 +13,166 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
-  <si>
-    <t xml:space="preserve">Stock Summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{company_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product: {{product_id.1.}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location: {{location_id.1.}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From {{date_from}} to {{date_to}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incoming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outgoing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lot / Serial Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UoM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{#each lines}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{prod_code}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{prod_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{lot_num}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{loc_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{cont_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{uom_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency open_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency open_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency open_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency period_in_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency  period_in_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency  period_in_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency period_out_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency  period_out_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency  period_out_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency close_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency close_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency close_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{/each}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_open_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_open_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_open_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_in_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_in_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_in_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_out_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_out_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_period_out_qty2}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_close_qty}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_close_amt}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_close_qty2}}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+  <si>
+    <t>Stock Summary</t>
+  </si>
+  <si>
+    <t>{{company_name}}</t>
+  </si>
+  <si>
+    <t>Product: {{product_id.1.}}</t>
+  </si>
+  <si>
+    <t>Location: {{location_id.1.}}</t>
+  </si>
+  <si>
+    <t>From {{date_from}} to {{date_to}}</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Incoming</t>
+  </si>
+  <si>
+    <t>Outgoing</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Brand</t>
+  </si>
+  <si>
+    <t>Lot / Serial Number</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>UoM</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Secondary Qty</t>
+  </si>
+  <si>
+    <t>{{#each lines}}</t>
+  </si>
+  <si>
+    <t>{{prod_code}}</t>
+  </si>
+  <si>
+    <t>{{prod_name}}</t>
+  </si>
+  <si>
+    <t>{{prod_brand}}</t>
+  </si>
+  <si>
+    <t>{{lot_num}}</t>
+  </si>
+  <si>
+    <t>{{loc_name}}</t>
+  </si>
+  <si>
+    <t>{{cont_name}}</t>
+  </si>
+  <si>
+    <t>{{uom_name}}</t>
+  </si>
+  <si>
+    <t>{{currency open_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency open_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency open_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency period_in_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency  period_in_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency  period_in_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency period_out_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency  period_out_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency  period_out_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency close_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency close_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency close_qty2}}</t>
+  </si>
+  <si>
+    <t>{{/each}}</t>
+  </si>
+  <si>
+    <t>{{currency total_open_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency total_open_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency total_open_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_in_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_in_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_in_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_out_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_out_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency total_period_out_qty2}}</t>
+  </si>
+  <si>
+    <t>{{currency total_close_qty}}</t>
+  </si>
+  <si>
+    <t>{{currency total_close_amt}}</t>
+  </si>
+  <si>
+    <t>{{currency total_close_qty2}}</t>
   </si>
 </sst>
 </file>
@@ -179,7 +180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -296,84 +297,85 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" s="2" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F6" s="0"/>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="0"/>
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -391,7 +393,7 @@
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -404,7 +406,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>16</v>
@@ -413,7 +415,7 @@
         <v>17</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>16</v>
@@ -422,7 +424,7 @@
         <v>17</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>16</v>
@@ -430,122 +432,128 @@
       <c r="R7" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="S7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="N11" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="O11" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -570,6 +578,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -594,6 +605,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>